<commit_message>
calculo do efeito com a funcao pairwise em vez de escalc, pois essa considera um SE agrupado para estudos multiarm.
</commit_message>
<xml_diff>
--- a/data/tablenma_c.xlsx
+++ b/data/tablenma_c.xlsx
@@ -1,21 +1,134 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ufscbr-my.sharepoint.com/personal/tamires_martins_ufsc_br/Documents/PC LAB/DissAnalysis/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_0C6EFDCE8F79A8D366075C52F3871AF57651E6D9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE3C822B-BAA1-4F75-A11E-E13F61A0ED2D}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
+  <si>
+    <t>V1</t>
+  </si>
+  <si>
+    <t>V2</t>
+  </si>
+  <si>
+    <t>V3</t>
+  </si>
+  <si>
+    <t>V4</t>
+  </si>
+  <si>
+    <t>V5</t>
+  </si>
+  <si>
+    <t>V6</t>
+  </si>
+  <si>
+    <t>imipramina</t>
+  </si>
+  <si>
+    <t>-0.14 (-5.09;  4.81)</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>4.27 ( 1.64;  6.91)</t>
+  </si>
+  <si>
+    <t>1.49 ( -2.99;  5.98)</t>
+  </si>
+  <si>
+    <t>amitriptilina</t>
+  </si>
+  <si>
+    <t>1.10 (-3.86;  6.05)</t>
+  </si>
+  <si>
+    <t>1.96 ( -1.62;  5.53)</t>
+  </si>
+  <si>
+    <t>0.46 ( -4.64;  5.56)</t>
+  </si>
+  <si>
+    <t>nortriptilina</t>
+  </si>
+  <si>
+    <t>2.28 (-0.14;  4.70)</t>
+  </si>
+  <si>
+    <t>2.86 ( -2.79;  8.51)</t>
+  </si>
+  <si>
+    <t>1.37 ( -5.35;  8.08)</t>
+  </si>
+  <si>
+    <t>0.90 ( -4.65;  6.46)</t>
+  </si>
+  <si>
+    <t>fluoxetina</t>
+  </si>
+  <si>
+    <t>1.37 (-3.63;  6.37)</t>
+  </si>
+  <si>
+    <t>4.52 ( -1.13; 10.18)</t>
+  </si>
+  <si>
+    <t>3.03 ( -3.69;  9.75)</t>
+  </si>
+  <si>
+    <t>2.57 ( -2.99;  8.12)</t>
+  </si>
+  <si>
+    <t>1.66 ( -5.41;  8.73)</t>
+  </si>
+  <si>
+    <t>citalopram</t>
+  </si>
+  <si>
+    <t>-0.29 (-5.29;  4.71)</t>
+  </si>
+  <si>
+    <t>4.23 (  1.60;  6.87)</t>
+  </si>
+  <si>
+    <t>2.74 ( -1.75;  7.23)</t>
+  </si>
+  <si>
+    <t>2.28 ( -0.14;  4.70)</t>
+  </si>
+  <si>
+    <t>1.37 ( -3.63;  6.37)</t>
+  </si>
+  <si>
+    <t>-0.29 ( -5.29;  4.71)</t>
+  </si>
+  <si>
+    <t>veículo</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -63,11 +176,19 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -109,7 +230,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -141,9 +262,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -175,6 +314,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -350,235 +507,160 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>V1</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>V2</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>V3</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>V4</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>V5</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>V6</t>
-        </is>
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>imipramina</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>-0.14 (-5.51;  5.23)</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>.</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>.</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>.</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>4.46 ( 1.77;  7.16)</t>
-        </is>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>1.61 ( -3.23;  6.45)</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>amitriptilina</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>.</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>.</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>.</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>1.07 (-4.30;  6.44)</t>
-        </is>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2.31 ( -1.32;  5.94)</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>0.70 ( -4.72;  6.12)</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>nortriptilina</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>.</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>.</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>2.12 (-0.31;  4.55)</t>
-        </is>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>3.12 ( -2.90;  9.13)</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>1.50 ( -5.73;  8.74)</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>0.81 ( -5.09;  6.70)</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>fluoxetina</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>.</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>1.32 (-4.06;  6.69)</t>
-        </is>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>4.70 ( -1.31; 10.72)</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>3.09 ( -4.14; 10.33)</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>2.39 ( -3.51;  8.29)</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>1.59 ( -6.02;  9.19)</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>citalopram</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>-0.27 (-5.65;  5.10)</t>
-        </is>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" t="s">
+        <v>27</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>4.43 (  1.73;  7.13)</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>2.82 ( -2.02;  7.67)</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>2.12 ( -0.31;  4.55)</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>1.32 ( -4.06;  6.69)</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>-0.27 ( -5.65;  5.10)</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>veículo</t>
-        </is>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>